<commit_message>
upload on 2018-03-26, update Spring Assemble method
</commit_message>
<xml_diff>
--- a/JavaEE/Jee_SSH相关/SSH.xlsx
+++ b/JavaEE/Jee_SSH相关/SSH.xlsx
@@ -31554,12 +31554,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
       <t>Bean</t>
     </r>
     <r>
@@ -32548,151 +32542,6 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>若应用中有很多</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Bean</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>，会导致</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>XML</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>配置文件臃肿，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Java</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>从</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>JDK1.5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>以后提供了</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Annotation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>功能，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Spring 3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>中也定义了一系列的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Annotation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>，如：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -32776,7 +32625,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>，并且可以作用在任何层次，使用时只需要将该注解标注在相应类上即可</t>
+      <t>，并且可以作用在任何层次</t>
     </r>
     <r>
       <rPr>
@@ -33144,37 +32993,145 @@
       <rPr>
         <sz val="8"/>
         <color rgb="FF00B050"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>@Repository/@Service/@Constroller</t>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>虽然</t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
         <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>作用与</t>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>@Repository</t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
         <color rgb="FF00B050"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>@Component</t>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
         <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>相同，只不过用途更加清晰</t>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>@Service</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>@Constroller</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>功能与</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>@component</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>相同，但为了使标注本身用途更加清晰，通常使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>@Repository</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>@Service</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>@Constroller</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分别对实现类进行标注</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.</t>
     </r>
     <r>
       <rPr>
@@ -33232,16 +33189,16 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>的属性变量、属性的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Setter</t>
+      <t>的属性、属性的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Set</t>
     </r>
     <r>
       <rPr>
@@ -33478,24 +33435,6 @@
         <rFont val="Consolas"/>
         <charset val="134"/>
       </rPr>
-      <t>Spring</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>将</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
       <t>name</t>
     </r>
     <r>
@@ -33505,7 +33444,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>属性解析为</t>
+      <t>为</t>
     </r>
     <r>
       <rPr>
@@ -33541,7 +33480,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>属性解析为</t>
+      <t>为</t>
     </r>
     <r>
       <rPr>
@@ -33754,7 +33693,7 @@
         <rFont val="Consolas"/>
         <charset val="134"/>
       </rPr>
-      <t>@Autowired</t>
+      <t xml:space="preserve">@Autowired </t>
     </r>
     <r>
       <rPr>
@@ -33827,151 +33766,6 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>虽然</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>@Repository</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>@Service</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>@Constroller</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>功能与</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>@component</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>相同，但为了使标注本身用途更加清晰，通常使用</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>@Repository</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>@Service</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>@Constroller</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>分别对实现类进行标注</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">.
 </t>
     </r>
     <r>
@@ -36847,6 +36641,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
       <t>Spring</t>
     </r>
     <r>
@@ -45791,9 +45592,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="66">
     <font>
@@ -45893,7 +45694,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -45914,15 +45723,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -45936,6 +45739,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -45943,9 +45754,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -45959,8 +45777,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -45989,22 +45808,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -46014,23 +45817,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -46200,13 +46001,13 @@
     <font>
       <sz val="8"/>
       <color rgb="FF00B050"/>
-      <name val="Consolas"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF00B050"/>
-      <name val="宋体"/>
+      <name val="Consolas"/>
       <charset val="134"/>
     </font>
     <font>
@@ -46239,13 +46040,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46257,13 +46076,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46281,7 +46100,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46293,7 +46118,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46305,31 +46130,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46347,31 +46166,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46383,31 +46178,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46423,6 +46212,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -46433,11 +46234,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -46452,16 +46259,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -46483,6 +46290,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -46491,42 +46309,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -46538,10 +46339,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -46550,133 +46351,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -47517,8 +47318,8 @@
   <sheetPr/>
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="K11" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:K13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="L10" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
upload on 2018-04-08, update springmvc content
</commit_message>
<xml_diff>
--- a/JavaEE/Jee_SSH相关/SSH.xlsx
+++ b/JavaEE/Jee_SSH相关/SSH.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="24180" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118">
   <si>
     <r>
       <rPr>
@@ -606,6 +606,20 @@
         <charset val="134"/>
       </rPr>
       <t>类</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>16 Spring</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>事务管理</t>
     </r>
   </si>
   <si>
@@ -6533,6 +6547,296 @@
       </rPr>
       <t xml:space="preserve">.
 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>事务管理</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个接口：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+    PlatformTransactionManager
+    TransactionDefinition
+    TransactionStatus
+    XML</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>配置文件中配置事务的详细信息，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Spring</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>将这些信息封装到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>TransactionDefinition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>对象中，通过</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>PlatformTransactionManager</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>getTransaction()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>就可以获取代表事务状态的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>TransactionStatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>对象以进行下一步操作</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.
+Spring</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>事务管理有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>种：声明式事务管理和编程式事务管理</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>声明式事务管理：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>XML</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>配置文件中定义数据源事务管理器</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Bean(class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>DataSourceTransactionManager)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，然后将事务管理器注入到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>TransactionProxyFactoryBean</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>中，使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>TransactionProxyFactoryBean</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>生成代理进行事务管理</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.</t>
     </r>
   </si>
   <si>
@@ -12560,6 +12864,400 @@
       </rPr>
       <t>");
  }</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>配置文件：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> 
+ &lt;!-- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>引入外部配置文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt;
+ &lt;context:property-placeholder location="classpath:c3p0-db.properties" /&gt;
+ &lt;bean id="dataSource" class="com.mchange.v2.c3p0.ComboPooledDataSource"&gt;
+  &lt;property name="driverClass" value="${jdbc.driverClass}"&gt;&lt;/property&gt;
+  &lt;property name="jdbcUrl" value="${jdbc.jdbcUrl}"&gt;&lt;/property&gt;
+  &lt;property name="user" value="${jdbc.user}"&gt;&lt;/property&gt;
+  &lt;property name="password" value="${jdbc.password}"&gt;&lt;/property&gt;
+ &lt;/bean&gt;
+ &lt;bean id="jdbcTemplate" class="org.springframework.jdbc.core.JdbcTemplate"&gt;
+  &lt;property name="dataSource" ref="dataSource"&gt;&lt;/property&gt;
+ &lt;/bean&gt;
+ &lt;bean id="accountDao" class="dao.AccountDaoImpl"&gt;
+  &lt;property name="jdbcTemplate" ref="jdbcTemplate"&gt;&lt;/property&gt;
+ &lt;/bean&gt;
+ &lt;bean id="accountService" class="service.AccountServiceImpl"&gt;
+  &lt;property name="accountDao" ref="accountDao"&gt;&lt;/property&gt;
+ &lt;/bean&gt;
+ &lt;!-- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>声明式事务管理定义</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数据源事务管理器</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>依赖于数据源</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt;
+ &lt;bean id="transactionManager" class="org.springframework.jdbc.datasource.DataSourceTransactionManager"&gt;
+  &lt;property name="dataSource" ref="dataSource"&gt;&lt;/property&gt;
+ &lt;/bean&gt;
+ &lt;!-- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>将数据源事务管理器注入到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> TransactionProxyFactoryBean </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>中</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>TransactionProxyFactoryBean</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>生成代理</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt;
+ &lt;bean id="accountServiceProxy" class="org.springframework.transaction.interceptor.TransactionProxyFactoryBean"&gt;
+  &lt;!-- transactionManager</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>依赖注入</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt;
+  &lt;property name="transactionManager" ref="transactionManager"&gt;&lt;/property&gt;
+  &lt;!-- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>设置需要进行事务管理的目标类</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt;
+  &lt;property name="target" ref="accountService"&gt;&lt;/property&gt;
+  &lt;!-- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>代理类需要实现的接口</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt;
+  &lt;property name="proxyInterfaces" value="service.AccountService"&gt;&lt;/property&gt;
+  &lt;!-- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>设置事务相关属性</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>给</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>TransactionDefinition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>赋值</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt;
+  &lt;property name="transactionAttributes"&gt;
+   &lt;props&gt;
+    &lt;!-- key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>表示对目标的哪些方法进行增强</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>, save*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>表示以</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>save</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>开头的方法</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, 
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>标签中的文本按照固定格式编写事务的详情及</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>TransactionDefinition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>内容</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt;
+    &lt;prop key="*"&gt;PROPAGATION_REQUIRED,ISOLATION_REPEATABLE_READ&lt;/prop&gt;
+   &lt;/props&gt;
+  &lt;/property&gt;
+ &lt;/bean&gt;</t>
     </r>
   </si>
   <si>
@@ -31554,6 +32252,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
       <t>Bean</t>
     </r>
     <r>
@@ -45592,9 +46296,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="66">
     <font>
@@ -45694,15 +46398,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -45723,9 +46426,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -45739,14 +46441,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -45754,16 +46448,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -45777,9 +46464,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -45808,6 +46494,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -45817,21 +46519,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -46040,13 +46744,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46058,31 +46780,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46100,13 +46822,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46118,25 +46852,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46154,43 +46870,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46202,13 +46882,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46220,7 +46924,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -46234,17 +46938,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -46259,16 +46957,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -46290,17 +46988,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -46309,25 +46996,42 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -46339,10 +47043,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -46351,31 +47055,31 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -46384,104 +47088,104 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -46530,8 +47234,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -47318,8 +48031,8 @@
   <sheetPr/>
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="L10" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10:L19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="O3" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -47335,12 +48048,12 @@
     <col min="10" max="10" width="54.1333333333333" style="1" customWidth="1"/>
     <col min="11" max="11" width="54.3166666666667" style="1" customWidth="1"/>
     <col min="12" max="14" width="54.225" style="1" customWidth="1"/>
-    <col min="15" max="15" width="45.0916666666667" style="1" customWidth="1"/>
+    <col min="15" max="15" width="76.725" style="1" customWidth="1"/>
     <col min="16" max="16" width="54.0333333333333" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" customHeight="1" spans="1:14">
+    <row r="1" ht="27" customHeight="1" spans="1:15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -47377,172 +48090,182 @@
       <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" ht="235" customHeight="1" spans="1:16">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="3" ht="300" customHeight="1" spans="1:14">
+    <row r="3" ht="300" customHeight="1" spans="1:15">
       <c r="A3" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="4" ht="348" customHeight="1" spans="1:14">
+    <row r="4" ht="348" customHeight="1" spans="1:15">
       <c r="A4" s="8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
-      <c r="M4" s="16" t="s">
-        <v>45</v>
+      <c r="M4" s="18" t="s">
+        <v>48</v>
       </c>
       <c r="N4" s="7"/>
+      <c r="O4" s="19"/>
     </row>
     <row r="5" ht="221" customHeight="1" spans="1:14">
       <c r="A5" s="12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="2"/>
       <c r="N5" s="7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" ht="193" customHeight="1" spans="1:14">
       <c r="A6" s="12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
@@ -47551,101 +48274,101 @@
     </row>
     <row r="7" ht="252" customHeight="1" spans="1:14">
       <c r="A7" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
-      <c r="M7" s="17" t="s">
-        <v>70</v>
+      <c r="M7" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="N7" s="7"/>
     </row>
     <row r="8" ht="214" customHeight="1" spans="1:14">
       <c r="A8" s="12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="17" t="s">
-        <v>75</v>
+      <c r="N8" s="20" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" ht="200" customHeight="1" spans="1:14">
       <c r="A9" s="12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="7"/>
     </row>
     <row r="10" ht="187" customHeight="1" spans="1:14">
       <c r="A10" s="12" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B10" s="2"/>
       <c r="H10" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N10" s="7"/>
     </row>
@@ -47653,36 +48376,36 @@
       <c r="A11" s="12"/>
       <c r="B11" s="2"/>
       <c r="F11" s="14" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
-      <c r="K11" s="17" t="s">
-        <v>93</v>
+      <c r="K11" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="7" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="N11" s="7"/>
     </row>
     <row r="12" ht="214" customHeight="1" spans="1:13">
       <c r="A12" s="15" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B12" s="2"/>
       <c r="F12" s="7" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="7"/>
@@ -47691,14 +48414,14 @@
     </row>
     <row r="13" ht="220" customHeight="1" spans="1:13">
       <c r="A13" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B13" s="2"/>
       <c r="F13" s="7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -47706,71 +48429,71 @@
     </row>
     <row r="14" ht="182" customHeight="1" spans="1:13">
       <c r="A14" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
     <row r="15" ht="202" customHeight="1" spans="1:13">
       <c r="A15" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="7" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" ht="174" customHeight="1" spans="1:12">
       <c r="A16" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="L16" s="7"/>
     </row>
     <row r="17" ht="129" customHeight="1" spans="1:12">
       <c r="A17" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="L17" s="7"/>
     </row>
     <row r="18" ht="360" customHeight="1" spans="1:12">
       <c r="A18" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="J18" s="7"/>
       <c r="L18" s="7"/>
     </row>
     <row r="19" ht="408" customHeight="1" spans="1:12">
       <c r="A19" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J19" s="7"/>
       <c r="L19" s="7"/>
     </row>
     <row r="20" ht="249" customHeight="1" spans="1:1">
       <c r="A20" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="J11:J12"/>
@@ -47788,6 +48511,7 @@
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="N5:N7"/>
     <mergeCell ref="N8:N10"/>
+    <mergeCell ref="O3:O4"/>
   </mergeCells>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>